<commit_message>
Jan 8 - Make Directory Updates
</commit_message>
<xml_diff>
--- a/gr/Input_Output/PixelValidation/pixel_testdata.xlsx
+++ b/gr/Input_Output/PixelValidation/pixel_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\PixelValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012F2D32-FC1C-499D-8659-0B81C526B90E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A0B85-5EA2-49D0-B428-C05682A2F296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="120">
   <si>
     <t>Test Run Environment</t>
   </si>
@@ -278,9 +278,6 @@
     <t>AccessiBe,Bing,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAdwordsRemarketing,GoogleAnalytics,LinkShare,Omniture,Pingdom</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,Cake,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,IncrementalMedia,LinkShare,Omniture,Pinterest,PowerInbox,Rejoiner</t>
-  </si>
-  <si>
     <t>BodyFirm</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>AccessiBe,Bing,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Hotjar,Kenshoo,Mouseflow,Omniture,Pingdom,Rejoiner,Smarter HQ,StackAdapt</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,Cake,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,Hotjar,IncrementalMedia,LinkShare,Mouseflow,Omniture,Outbrain,Pinterest,PowerInbox,PropelMedia,Rejoiner,w55c</t>
-  </si>
-  <si>
     <t>AccessiBe,Bing,Cake,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Kenshoo,Mouseflow,Omniture,Rejoiner</t>
   </si>
   <si>
@@ -387,6 +381,15 @@
   </si>
   <si>
     <t>AccessiBe,Bing,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Iconmedia,Mouseflow,Omniture,PayPal,Pingdom,RadianceLabs,Sailthru,Smarter HQ,w55c</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,Cake,CJ,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,IncrementalMedia,LinkShare,Omniture,Pinterest,PowerInbox,Rejoiner</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,Cake,CJ,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,Hotjar,IncrementalMedia,LinkShare,Mouseflow,Omniture,Outbrain,Pinterest,PowerInbox,PropelMedia,Rejoiner,w55c</t>
+  </si>
+  <si>
+    <t>Rejoiner</t>
   </si>
 </sst>
 </file>
@@ -862,7 +865,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -900,299 +903,18 @@
         <v>56</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
+      <c r="E2" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>85</v>
+      <c r="A3" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1216,8 +938,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,16 +973,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>18</v>
@@ -1277,7 +999,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1294,7 +1016,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1311,7 +1033,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
@@ -1352,7 +1074,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1369,7 +1091,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1437,7 +1159,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,7 +1176,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,7 +1193,7 @@
         <v>50</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1488,7 +1210,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1522,7 +1244,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,7 +1261,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1547,16 +1269,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1564,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>18</v>
@@ -1573,7 +1295,7 @@
         <v>50</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1581,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>18</v>
@@ -1590,7 +1312,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,7 +1407,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:E91"/>
+      <selection activeCell="A73" sqref="A73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1463,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>50</v>
@@ -2838,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>18</v>
@@ -2856,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>18</v>
@@ -2874,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>18</v>
@@ -2892,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>18</v>
@@ -2930,7 +2652,7 @@
         <v>56</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>50</v>
@@ -3233,7 +2955,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>18</v>
@@ -3253,7 +2975,7 @@
         <v>19</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>50</v>
@@ -3270,7 +2992,7 @@
         <v>5</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>50</v>
@@ -3400,61 +3122,61 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C104" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C105" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C106" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C107" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>109</v>
+      </c>
+      <c r="C109" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C110" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C111" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C114" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C115" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jan 29 - Pixel testdata update
</commit_message>
<xml_diff>
--- a/gr/Input_Output/PixelValidation/pixel_testdata.xlsx
+++ b/gr/Input_Output/PixelValidation/pixel_testdata.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\PixelValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A0B85-5EA2-49D0-B428-C05682A2F296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBBE08D-8AE6-4857-AEC5-A89432186197}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Run Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Data" sheetId="2" r:id="rId2"/>
-    <sheet name="FB Pixel Test data" sheetId="5" r:id="rId3"/>
+    <sheet name="FBPixels" sheetId="6" r:id="rId1"/>
+    <sheet name="AllPixels" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Data" sheetId="2" r:id="rId3"/>
+    <sheet name="FB Pixel Test data" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="108">
   <si>
     <t>Test Run Environment</t>
   </si>
@@ -206,9 +208,6 @@
     <t>Bing,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,Omniture</t>
   </si>
   <si>
-    <t>Bing,Cake,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Hotjar,Omniture,Rejoiner</t>
-  </si>
-  <si>
     <t>crepeerase</t>
   </si>
   <si>
@@ -287,9 +286,6 @@
     <t>End</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,Cake,Criteo,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,Hotjar,Kenshoo,Mouseflow,Omniture,Pingdom,Rejoiner,Smarter HQ</t>
-  </si>
-  <si>
     <t>AccessiBe,Bing,Cake,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAdwordsRemarketing,GoogleAnalytics,HarmonyConversionTracking,Kenshoo,LinkShare,Mouseflow,Omniture,Pingdom</t>
   </si>
   <si>
@@ -302,27 +298,18 @@
     <t>AccessiBe,Bing,Cake,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Justuno,Kenshoo,Mouseflow,Omniture</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Hotjar,Kenshoo,Mouseflow,Omniture,Pingdom,Rejoiner,Smarter HQ,StackAdapt</t>
-  </si>
-  <si>
     <t>AccessiBe,Bing,Cake,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Kenshoo,Mouseflow,Omniture,Rejoiner</t>
   </si>
   <si>
     <t>BodyFirm-SpotFade</t>
   </si>
   <si>
-    <t>AccessiBe,AmazonFire,Bing,Cake,Criteo,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAdwordsRemarketing,GoogleAnalytics,HarmonyConversionTracking,Hotjar,Kenshoo,Mouseflow,IncrementalMedia,LinkShare,Omniture,Outbrain,Pingdom,Pinterest,PropelMedia,Rejoiner,Smarter HQ,StackAdapt,StarMobile,Taboola,tvpixel,w55c</t>
-  </si>
-  <si>
     <t>SpotFade</t>
   </si>
   <si>
     <t>Bing,Cake,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Mouseflow,Omniture,Rakuten</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,Cake,Criteo,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Hotjar,Kenshoo,Mouseflow,Omniture,Rejoiner,Smarter HQ</t>
-  </si>
-  <si>
     <t>AllKind</t>
   </si>
   <si>
@@ -344,39 +331,6 @@
     <t>advanceddeluxe20offevergreensale</t>
   </si>
   <si>
-    <t>deluxe20off-60secondeye</t>
-  </si>
-  <si>
-    <t>wy</t>
-  </si>
-  <si>
-    <t>deluxe20off-holiday</t>
-  </si>
-  <si>
-    <t>deluxe20off-fcp</t>
-  </si>
-  <si>
-    <t>mb5-deluxe20offb15</t>
-  </si>
-  <si>
-    <t>mb</t>
-  </si>
-  <si>
-    <t>mb7deluxe20offb15</t>
-  </si>
-  <si>
-    <t>core</t>
-  </si>
-  <si>
-    <t>ce</t>
-  </si>
-  <si>
-    <t>advanced-holiday-special</t>
-  </si>
-  <si>
-    <t>classic-deluxe20off-holiday</t>
-  </si>
-  <si>
     <t>JLoBeauty</t>
   </si>
   <si>
@@ -386,10 +340,22 @@
     <t>AccessiBe,Bing,Cake,CJ,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,IncrementalMedia,LinkShare,Omniture,Pinterest,PowerInbox,Rejoiner</t>
   </si>
   <si>
-    <t>AccessiBe,Bing,Cake,CJ,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,Hotjar,IncrementalMedia,LinkShare,Mouseflow,Omniture,Outbrain,Pinterest,PowerInbox,PropelMedia,Rejoiner,w55c</t>
-  </si>
-  <si>
-    <t>Rejoiner</t>
+    <t>AccessiBe,AmazonFire,Bing,Cake,Criteo,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAdwordsRemarketing,GoogleAnalytics,HarmonyConversionTracking,Kenshoo,Mouseflow,IncrementalMedia,LinkShare,Omniture,Outbrain,Pingdom,Pinterest,PropelMedia,Rejoiner,Smarter HQ,StackAdapt,StarMobile,Taboola,tvpixel,w55c</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Kenshoo,Mouseflow,Omniture,Pingdom,Rejoiner,Smarter HQ,StackAdapt</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,Cake,Criteo,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,Kenshoo,Mouseflow,Omniture,Pingdom,Rejoiner,Smarter HQ</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,Cake,CJ,DoubleclickFloodlight,DoubleclickFloodlightConfirmation,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,HarmonyConversionTracking,IncrementalMedia,LinkShare,Mouseflow,Omniture,Outbrain,Pinterest,PowerInbox,PropelMedia,Rejoiner,w55c</t>
+  </si>
+  <si>
+    <t>AccessiBe,Bing,Cake,Criteo,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Kenshoo,Mouseflow,Omniture,Rejoiner,Smarter HQ</t>
+  </si>
+  <si>
+    <t>Bing,Cake,DoubleclickFloodlightConfirmationnew,Facebook,GoogleAdwordsConversionTracking,GoogleAnalytics,Omniture,Rejoiner</t>
   </si>
 </sst>
 </file>
@@ -863,9 +829,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCBB41D-A12A-4622-9C42-DCD0E274A75A}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -908,13 +873,362 @@
       <c r="D2" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="86.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="E2" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -933,13 +1247,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,16 +1287,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -990,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>18</v>
@@ -999,7 +1313,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1016,7 +1330,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1033,7 +1347,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
@@ -1074,7 +1388,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1091,7 +1405,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1108,7 +1422,7 @@
         <v>50</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,7 +1439,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1456,7 @@
         <v>50</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1159,7 +1473,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1176,7 +1490,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,7 +1507,7 @@
         <v>50</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1210,7 +1524,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1227,7 +1541,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1244,7 +1558,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1261,7 +1575,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1269,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>18</v>
@@ -1278,7 +1592,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>18</v>
@@ -1295,7 +1609,7 @@
         <v>50</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1303,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>18</v>
@@ -1312,7 +1626,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,13 +1715,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:E73"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,7 +1777,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>50</v>
@@ -1481,7 +1795,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>50</v>
@@ -1661,7 +1975,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>50</v>
@@ -1861,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>50</v>
@@ -1879,7 +2193,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>50</v>
@@ -1897,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>50</v>
@@ -1915,7 +2229,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>50</v>
@@ -1933,7 +2247,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>50</v>
@@ -2041,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>50</v>
@@ -2059,7 +2373,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>50</v>
@@ -2077,7 +2391,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>50</v>
@@ -2095,7 +2409,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>50</v>
@@ -2113,7 +2427,7 @@
         <v>9</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>50</v>
@@ -2131,7 +2445,7 @@
         <v>9</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>50</v>
@@ -2149,7 +2463,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>50</v>
@@ -2275,7 +2589,7 @@
         <v>19</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>50</v>
@@ -2293,7 +2607,7 @@
         <v>19</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>50</v>
@@ -2383,7 +2697,7 @@
         <v>34</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>50</v>
@@ -2401,7 +2715,7 @@
         <v>34</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>50</v>
@@ -2473,7 +2787,7 @@
         <v>34</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>50</v>
@@ -2491,7 +2805,7 @@
         <v>34</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>50</v>
@@ -2560,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>18</v>
@@ -2578,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>18</v>
@@ -2596,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>18</v>
@@ -2614,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>18</v>
@@ -2652,7 +2966,7 @@
         <v>56</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>50</v>
@@ -2669,7 +2983,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>50</v>
@@ -2805,7 +3119,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>50</v>
@@ -2907,7 +3221,7 @@
         <v>34</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>50</v>
@@ -2924,7 +3238,7 @@
         <v>34</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>50</v>
@@ -2955,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>18</v>
@@ -2975,7 +3289,7 @@
         <v>19</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>50</v>
@@ -2992,7 +3306,7 @@
         <v>5</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>50</v>
@@ -3077,7 +3391,7 @@
         <v>9</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>50</v>
@@ -3121,62 +3435,326 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>105</v>
-      </c>
-      <c r="C104" t="s">
-        <v>111</v>
+      <c r="A104" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C105" s="13" t="s">
-        <v>104</v>
+      <c r="A105" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C106" s="13" t="s">
-        <v>106</v>
+      <c r="A106" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C107" s="13" t="s">
-        <v>107</v>
+      <c r="A107" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>109</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>111</v>
+      <c r="A109" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C110" s="13" t="s">
-        <v>108</v>
+      <c r="A110" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C111" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>112</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="13" t="s">
-        <v>114</v>
+      <c r="A111" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E122" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>